<commit_message>
clean up exams-data folder
</commit_message>
<xml_diff>
--- a/exams-data/ingest-log.xlsx
+++ b/exams-data/ingest-log.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="inject-log" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'inject-log'!$A$1:$D$55</definedName>
+  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -19,14 +22,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>https://www.sqa.org.uk/sqa/files_ccc/ExamTimetable2020.pdf</t>
   </si>
   <si>
-    <t>exams sqa 2018.csv</t>
-  </si>
-  <si>
     <t>Ingest</t>
   </si>
   <si>
@@ -48,24 +48,15 @@
     <t>https://filestore.aqa.org.uk/admin/t_table_pdf/AQA-TT-GCSE-JUN20-CONFIRMED.PDF</t>
   </si>
   <si>
-    <t>AQA Exams - 2020.xlsx</t>
-  </si>
-  <si>
     <t>https://qualifications.pearson.com/content/dam/pdf/Support/Examination-timetables-for-UK-Edexcel-GCSE/GCSE-Final-2006.xlsx</t>
   </si>
   <si>
     <t>I102</t>
   </si>
   <si>
-    <t>Edexcel GCSE Exams - 2020.xlsx</t>
-  </si>
-  <si>
     <t>I103</t>
   </si>
   <si>
-    <t>Edexcel A Level Exams - 2020.xlsx</t>
-  </si>
-  <si>
     <t>https://qualifications.pearson.com/content/dam/pdf/Support/Examination-timetables/GCE-Final-2006.xlsx</t>
   </si>
   <si>
@@ -81,19 +72,163 @@
     <t>https://ccea.org.uk/downloads/docs/ccea-asset/Examinations/Final%20GCSE%20Timetable%20Summer%202020.pdf</t>
   </si>
   <si>
-    <t>CEA GCSE Exams - 2020.xlsx</t>
-  </si>
-  <si>
     <t>I106</t>
   </si>
   <si>
-    <t>WJEC+Educas GCSE Exams - 2020.xslx</t>
-  </si>
-  <si>
-    <t>OCR Exams - 2020.xlsx</t>
-  </si>
-  <si>
     <t>https://www.wjec.co.uk/exam-officers/Examination_Timetable_2020_Final_update_041219%20(2).pdf?language_id=1</t>
+  </si>
+  <si>
+    <t>2020/WJEC GCSE Exams - 2020.xslx</t>
+  </si>
+  <si>
+    <t>2020/CEA GCSE Exams - 2020.xlsx</t>
+  </si>
+  <si>
+    <t>2020/OCR Exams - 2020.xlsx</t>
+  </si>
+  <si>
+    <t>2020/Edexcel GCE Exams - 2020.xlsx</t>
+  </si>
+  <si>
+    <t>2020/Edexcel GCSE Exams - 2020.xlsx</t>
+  </si>
+  <si>
+    <t>2020/AQA Exams - 2020.xlsx</t>
+  </si>
+  <si>
+    <t>2020/SQA Exams - 2020.xlsx</t>
+  </si>
+  <si>
+    <t>./2018/Exams 2018 - AQA Exams Summer 2018.csv</t>
+  </si>
+  <si>
+    <t>./2018/Exams 2018 - CEA GCE Summer 2018.csv</t>
+  </si>
+  <si>
+    <t>./2018/Exams 2018 - CEA GCSE Summer 2018.csv</t>
+  </si>
+  <si>
+    <t>./2018/exams edexcel 2018.csv</t>
+  </si>
+  <si>
+    <t>./2018/exams edexcel 2018.xls</t>
+  </si>
+  <si>
+    <t>./2018/exams edexcel 2018.xlsx</t>
+  </si>
+  <si>
+    <t>./2018/exams ocr 2018.csv</t>
+  </si>
+  <si>
+    <t>./2018/exams ocr 2018.xlsx</t>
+  </si>
+  <si>
+    <t>./2018/exams sqa 2018.csv</t>
+  </si>
+  <si>
+    <t>./2018/exams sqa 2018.xlsx</t>
+  </si>
+  <si>
+    <t>./2018/exams wjec cbac 2018.csv</t>
+  </si>
+  <si>
+    <t>./2018/exams wjec cbac 2018.xlsx</t>
+  </si>
+  <si>
+    <t>./2019/Exams 2019 - AQA Exams Summer 2019.csv</t>
+  </si>
+  <si>
+    <t>./2019/Exams 2019 - CEA Exams January 2019.csv</t>
+  </si>
+  <si>
+    <t>./2019/Exams 2019 - CEA Exams March 2019.csv</t>
+  </si>
+  <si>
+    <t>./2019/Exams 2019 - CEA Exams Summer 2019.csv</t>
+  </si>
+  <si>
+    <t>./2019/Exams 2019 - Edexcel GCSE Mayâ€“June 2019.csv</t>
+  </si>
+  <si>
+    <t>./2019/Exams 2019 - OCR GCSE Jun 2019.csv</t>
+  </si>
+  <si>
+    <t>./2019/Exams 2019 - OCR Nationals and Technicals Jan 2019.csv</t>
+  </si>
+  <si>
+    <t>./2019/Exams 2019 - SQA Summer 2019.csv</t>
+  </si>
+  <si>
+    <t>./2019/Exams 2019 - WJEC Eduqas Nov 2018-Jan 2019.csv</t>
+  </si>
+  <si>
+    <t>./2019/Exams 2019 - WJEC Eduqas Summer 2019.csv</t>
+  </si>
+  <si>
+    <t>I001</t>
+  </si>
+  <si>
+    <t>I002</t>
+  </si>
+  <si>
+    <t>I003</t>
+  </si>
+  <si>
+    <t>I004</t>
+  </si>
+  <si>
+    <t>I005</t>
+  </si>
+  <si>
+    <t>I006</t>
+  </si>
+  <si>
+    <t>I007</t>
+  </si>
+  <si>
+    <t>I008</t>
+  </si>
+  <si>
+    <t>I009</t>
+  </si>
+  <si>
+    <t>I010</t>
+  </si>
+  <si>
+    <t>I011</t>
+  </si>
+  <si>
+    <t>I012</t>
+  </si>
+  <si>
+    <t>I050</t>
+  </si>
+  <si>
+    <t>I051</t>
+  </si>
+  <si>
+    <t>I052</t>
+  </si>
+  <si>
+    <t>I053</t>
+  </si>
+  <si>
+    <t>I054</t>
+  </si>
+  <si>
+    <t>I055</t>
+  </si>
+  <si>
+    <t>I056</t>
+  </si>
+  <si>
+    <t>I057</t>
+  </si>
+  <si>
+    <t>I058</t>
+  </si>
+  <si>
+    <t>I059</t>
   </si>
 </sst>
 </file>
@@ -103,7 +238,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -127,6 +262,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -136,7 +279,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -144,8 +287,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -161,13 +313,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="18">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -177,6 +334,9 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -511,137 +671,314 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="53.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="107" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="3" customFormat="1" ht="16" thickBot="1">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2">
-        <v>43861</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="2">
-        <v>43861</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2">
-        <v>43861</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="2">
-        <v>43861</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="2">
-        <v>43863</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="2">
-        <v>43862</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2">
+        <v>43861</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="2">
+        <v>43861</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="2">
+        <v>43861</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="2">
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="2">
+        <v>43861</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="2">
         <v>43863</v>
       </c>
     </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="2">
+        <v>43862</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="2">
+        <v>43863</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:D55"/>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="C6" r:id="rId2"/>
-    <hyperlink ref="C7" r:id="rId3"/>
-    <hyperlink ref="C8" r:id="rId4"/>
+    <hyperlink ref="C25" r:id="rId1"/>
+    <hyperlink ref="C28" r:id="rId2"/>
+    <hyperlink ref="C29" r:id="rId3"/>
+    <hyperlink ref="C30" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>